<commit_message>
TMT0072159_TMT0072162_VerifyBankerCanCreateExternalAndInternalFollowUpActivity - Final - 3 sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyBankerCanCreateExternalAndInternalFollowUpActivity.xlsx
+++ b/TestData/TMTC0032668_VerifyBankerCanCreateExternalAndInternalFollowUpActivity.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD515DC-F537-4672-BAC8-BF3A4086E6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C05AB1C-1EE8-4C3C-A974-7C2D5A4E3850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="Contact" sheetId="10" r:id="rId2"/>
     <sheet name="Activity" sheetId="11" r:id="rId3"/>
+    <sheet name="Followup" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Users</t>
   </si>
@@ -110,6 +111,21 @@
   </si>
   <si>
     <t>Internal FollowUp Meeting Description</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>External Followup</t>
+  </si>
+  <si>
+    <t>Internal Followup</t>
   </si>
 </sst>
 </file>
@@ -518,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,4 +623,43 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FD42B5-FCC0-46AF-9C9E-BDDDE197E6BE}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed Test Data for LV Activities - 16 Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyBankerCanCreateExternalAndInternalFollowUpActivity.xlsx
+++ b/TestData/TMTC0032668_VerifyBankerCanCreateExternalAndInternalFollowUpActivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C05AB1C-1EE8-4C3C-A974-7C2D5A4E3850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AAA7C4-A3B9-4BF3-8A9B-6FF370062EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Users</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Thomas Bailey</t>
   </si>
   <si>
-    <t>StandardTestCompany</t>
-  </si>
-  <si>
     <t>ContactName</t>
   </si>
   <si>
@@ -126,6 +123,12 @@
   </si>
   <si>
     <t>Internal Followup</t>
+  </si>
+  <si>
+    <t>Activity Test External Contact</t>
+  </si>
+  <si>
+    <t>ActivityCompany</t>
   </si>
 </sst>
 </file>
@@ -492,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,10 +507,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>12</v>
@@ -515,10 +518,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -577,7 +580,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -586,7 +589,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -600,7 +603,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -609,10 +612,10 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -629,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FD42B5-FCC0-46AF-9C9E-BDDDE197E6BE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -640,23 +643,23 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>